<commit_message>
Updated new functionalities in fit_and_augment class. Also, aligned the use of solve_ivp and odeint.
</commit_message>
<xml_diff>
--- a/examples/data/batch_batch1_testing_batchdata.xlsx
+++ b/examples/data/batch_batch1_testing_batchdata.xlsx
@@ -463,10 +463,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1294396932959941</v>
+        <v>0.3438530600655295</v>
       </c>
       <c r="D2" t="n">
-        <v>85.97371648230884</v>
+        <v>50.9346037455865</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -480,13 +480,13 @@
         <v>4.210526315789473</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2076535069114193</v>
+        <v>0.4825802292055428</v>
       </c>
       <c r="D3" t="n">
-        <v>84.85637628780276</v>
+        <v>48.95278704358631</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1865958124825144</v>
+        <v>0.330963389234032</v>
       </c>
     </row>
     <row r="4">
@@ -497,13 +497,13 @@
         <v>8.421052631578947</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3315484433631548</v>
+        <v>0.6697017583665801</v>
       </c>
       <c r="D4" t="n">
-        <v>83.08644862420654</v>
+        <v>46.27962234128579</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4821737323030834</v>
+        <v>0.7773818945182209</v>
       </c>
     </row>
     <row r="5">
@@ -514,13 +514,13 @@
         <v>12.63157894736842</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5253553379585646</v>
+        <v>0.9151453693242683</v>
       </c>
       <c r="D5" t="n">
-        <v>80.31777870141499</v>
+        <v>42.77328504189024</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9445416094092752</v>
+        <v>1.362940223517277</v>
       </c>
     </row>
     <row r="6">
@@ -531,13 +531,13 @@
         <v>16.84210526315789</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8224605018333396</v>
+        <v>1.224914635269494</v>
       </c>
       <c r="D6" t="n">
-        <v>76.07341921748962</v>
+        <v>38.34800981410131</v>
       </c>
       <c r="E6" t="n">
-        <v>1.65334964322481</v>
+        <v>2.101961186558029</v>
       </c>
     </row>
     <row r="7">
@@ -548,13 +548,13 @@
         <v>21.05263157894737</v>
       </c>
       <c r="C7" t="n">
-        <v>1.263411897844627</v>
+        <v>1.596051013944228</v>
       </c>
       <c r="D7" t="n">
-        <v>69.7741135601855</v>
+        <v>33.0460615473194</v>
       </c>
       <c r="E7" t="n">
-        <v>2.705333687994596</v>
+        <v>2.987386547110608</v>
       </c>
     </row>
     <row r="8">
@@ -565,13 +565,13 @@
         <v>25.26315789473684</v>
       </c>
       <c r="C8" t="n">
-        <v>1.885020863059941</v>
+        <v>2.011526501780981</v>
       </c>
       <c r="D8" t="n">
-        <v>60.89398548568101</v>
+        <v>27.11069743536578</v>
       </c>
       <c r="E8" t="n">
-        <v>4.188315076436845</v>
+        <v>3.978592353806863</v>
       </c>
     </row>
     <row r="9">
@@ -582,13 +582,13 @@
         <v>29.47368421052632</v>
       </c>
       <c r="C9" t="n">
-        <v>2.693529737658339</v>
+        <v>2.439016549222489</v>
       </c>
       <c r="D9" t="n">
-        <v>49.34385870570391</v>
+        <v>21.00369675762995</v>
       </c>
       <c r="E9" t="n">
-        <v>6.117186248693023</v>
+        <v>4.998461466988747</v>
       </c>
     </row>
     <row r="10">
@@ -599,13 +599,13 @@
         <v>33.68421052631579</v>
       </c>
       <c r="C10" t="n">
-        <v>3.624791330147982</v>
+        <v>2.837881536945993</v>
       </c>
       <c r="D10" t="n">
-        <v>36.04012167013759</v>
+        <v>15.30562550443704</v>
       </c>
       <c r="E10" t="n">
-        <v>8.338910333632597</v>
+        <v>5.950039366271963</v>
       </c>
     </row>
     <row r="11">
@@ -616,13 +616,13 @@
         <v>37.89473684210526</v>
       </c>
       <c r="C11" t="n">
-        <v>4.529107093435749</v>
+        <v>3.173379749207618</v>
       </c>
       <c r="D11" t="n">
-        <v>23.12132505174092</v>
+        <v>10.51279390069954</v>
       </c>
       <c r="E11" t="n">
-        <v>10.49634936890484</v>
+        <v>6.750442244096125</v>
       </c>
     </row>
     <row r="12">
@@ -633,13 +633,13 @@
         <v>42.10526315789473</v>
       </c>
       <c r="C12" t="n">
-        <v>5.240658897767408</v>
+        <v>3.429012208198724</v>
       </c>
       <c r="D12" t="n">
-        <v>12.95629927557438</v>
+        <v>6.860901629398032</v>
       </c>
       <c r="E12" t="n">
-        <v>12.19390867352466</v>
+        <v>7.360308253403478</v>
       </c>
     </row>
     <row r="13">
@@ -650,13 +650,13 @@
         <v>46.31578947368421</v>
       </c>
       <c r="C13" t="n">
-        <v>5.693150829998912</v>
+        <v>3.608050188682537</v>
       </c>
       <c r="D13" t="n">
-        <v>6.492128815124324</v>
+        <v>4.303216193914981</v>
       </c>
       <c r="E13" t="n">
-        <v>13.27342514041982</v>
+        <v>7.787441721129148</v>
       </c>
     </row>
     <row r="14">
@@ -667,13 +667,13 @@
         <v>50.52631578947368</v>
       </c>
       <c r="C14" t="n">
-        <v>5.935920177477171</v>
+        <v>3.725594175089091</v>
       </c>
       <c r="D14" t="n">
-        <v>3.023995279720622</v>
+        <v>2.624016388107058</v>
       </c>
       <c r="E14" t="n">
-        <v>13.85260344083223</v>
+        <v>8.067868088699072</v>
       </c>
     </row>
     <row r="15">
@@ -684,13 +684,13 @@
         <v>54.73684210526316</v>
       </c>
       <c r="C15" t="n">
-        <v>6.052834252301664</v>
+        <v>3.799339808000172</v>
       </c>
       <c r="D15" t="n">
-        <v>1.353794210799295</v>
+        <v>1.570507346520189</v>
       </c>
       <c r="E15" t="n">
-        <v>14.1315270193421</v>
+        <v>8.243804098644079</v>
       </c>
     </row>
     <row r="16">
@@ -701,13 +701,13 @@
         <v>58.94736842105263</v>
       </c>
       <c r="C16" t="n">
-        <v>6.105981495155647</v>
+        <v>3.844246665071113</v>
       </c>
       <c r="D16" t="n">
-        <v>0.5945478843138013</v>
+        <v>0.9289808169353263</v>
       </c>
       <c r="E16" t="n">
-        <v>14.25832115586518</v>
+        <v>8.350939029084749</v>
       </c>
     </row>
     <row r="17">
@@ -718,13 +718,13 @@
         <v>63.1578947368421</v>
       </c>
       <c r="C17" t="n">
-        <v>6.129481412492744</v>
+        <v>3.87108503956683</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2588347794981508</v>
+        <v>0.5455754669965129</v>
       </c>
       <c r="E17" t="n">
-        <v>14.31438524436939</v>
+        <v>8.414967722524532</v>
       </c>
     </row>
     <row r="18">
@@ -735,13 +735,13 @@
         <v>67.36842105263158</v>
       </c>
       <c r="C18" t="n">
-        <v>6.139742511593304</v>
+        <v>3.886942998941307</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1122476494901516</v>
+        <v>0.3190331902182707</v>
       </c>
       <c r="E18" t="n">
-        <v>14.33886529508072</v>
+        <v>8.452800282746498</v>
       </c>
     </row>
     <row r="19">
@@ -752,13 +752,13 @@
         <v>71.57894736842105</v>
       </c>
       <c r="C19" t="n">
-        <v>6.144198149853797</v>
+        <v>3.896249335110733</v>
       </c>
       <c r="D19" t="n">
-        <v>0.04859567434024974</v>
+        <v>0.1860855306550447</v>
       </c>
       <c r="E19" t="n">
-        <v>14.34949517493076</v>
+        <v>8.475002541893558</v>
       </c>
     </row>
     <row r="20">
@@ -769,13 +769,13 @@
         <v>75.78947368421052</v>
       </c>
       <c r="C20" t="n">
-        <v>6.146128222095857</v>
+        <v>3.901688867334186</v>
       </c>
       <c r="D20" t="n">
-        <v>0.02102321373937761</v>
+        <v>0.1083779274628423</v>
       </c>
       <c r="E20" t="n">
-        <v>14.3540997758511</v>
+        <v>8.487979711626657</v>
       </c>
     </row>
     <row r="21">
@@ -786,13 +786,13 @@
         <v>80</v>
       </c>
       <c r="C21" t="n">
-        <v>6.146963402637169</v>
+        <v>3.904860756908391</v>
       </c>
       <c r="D21" t="n">
-        <v>0.009092063149217719</v>
+        <v>0.06306521925991308</v>
       </c>
       <c r="E21" t="n">
-        <v>14.35609227799966</v>
+        <v>8.495546933896545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>